<commit_message>
Se mejora base de datos para el ejercicio.
</commit_message>
<xml_diff>
--- a/Dataset/EjercicioLimpieza.xlsx
+++ b/Dataset/EjercicioLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE386AD-AAB5-4B0D-A620-F68B81553C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D2892A-208F-4F4C-BF00-CCD73ACA6BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>NA</t>
   </si>
@@ -37,9 +37,6 @@
     <t>01/05/2013</t>
   </si>
   <si>
-    <t>23/09/2014</t>
-  </si>
-  <si>
     <t>2/06/2014</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>02 02 17</t>
   </si>
   <si>
-    <t>18 02 06</t>
-  </si>
-  <si>
     <t>09 09 09</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>09 04 2019  3:01:36 a. m.</t>
   </si>
   <si>
-    <t>20 06 2019</t>
-  </si>
-  <si>
     <t>tipo-documento</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>Hijos</t>
-  </si>
-  <si>
     <t>Prom*Caridad</t>
   </si>
   <si>
@@ -197,6 +185,21 @@
   </si>
   <si>
     <t>Tiemp_Prom'</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>ninguna</t>
+  </si>
+  <si>
+    <t>2/19/2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02 18 06</t>
+  </si>
+  <si>
+    <t>06 20 2019</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -724,6 +727,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1081,53 +1087,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>103586998</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>103586998</v>
@@ -1136,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1153,13 +1156,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>103587812</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2">
         <v>103587812</v>
@@ -1168,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1183,7 +1186,7 @@
         <v>12100</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1194,7 +1197,7 @@
         <v>100730671</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13">
         <v>100730671</v>
@@ -1203,7 +1206,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
@@ -1218,18 +1221,18 @@
         <v>31100</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8">
         <v>19355635</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="8">
         <v>19355635</v>
@@ -1238,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7">
         <v>3</v>
@@ -1255,13 +1258,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>103857245</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2">
         <v>103857245</v>
@@ -1270,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -1287,13 +1290,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="13">
         <v>190730671</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="13">
         <v>190730671</v>
@@ -1302,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="12">
         <v>1</v>
@@ -1317,13 +1320,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>123488986</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>123488986</v>
@@ -1332,13 +1335,13 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
+      <c r="H8" t="s">
+        <v>56</v>
       </c>
       <c r="I8">
         <v>5</v>
@@ -1349,13 +1352,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2">
         <v>210216677</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2">
         <v>210216677</v>
@@ -1364,10 +1367,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -1381,13 +1384,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>39359318</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2">
         <v>39359318</v>
@@ -1396,13 +1399,13 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1413,13 +1416,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8">
         <v>19355635</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="8">
         <v>19355635</v>
@@ -1428,7 +1431,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="7">
         <v>3</v>
@@ -1445,22 +1448,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2">
         <v>32321157</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
         <v>32321157</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1469,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="J12">
         <v>34200</v>
@@ -1483,7 +1486,7 @@
         <v>127032350</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2">
         <v>127032350</v>
@@ -1492,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="16">
         <v>4</v>
@@ -1515,7 +1518,7 @@
         <v>39350897</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4">
         <v>39350897</v>
@@ -1524,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="3">
         <v>2</v>
@@ -1545,7 +1548,7 @@
         <v>60328769</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2">
         <v>60328769</v>
@@ -1554,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1571,7 +1574,7 @@
         <v>1035874914</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2">
         <v>1035874914</v>
@@ -1580,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1597,13 +1600,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="10">
         <v>32075905</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="10">
         <v>32075905</v>
@@ -1612,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="9">
         <v>2</v>
@@ -1629,13 +1632,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2">
         <v>1203870219</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2">
         <v>1203870219</v>
@@ -1644,7 +1647,7 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1661,13 +1664,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2">
         <v>70320453</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2">
         <v>70320453</v>
@@ -1676,7 +1679,7 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -1693,13 +1696,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4">
         <v>39350897</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="4">
         <v>39350897</v>
@@ -1708,7 +1711,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="3">
         <v>2</v>
@@ -1723,13 +1726,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>1040305449</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="2">
         <v>1040305449</v>
@@ -1738,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1755,25 +1758,25 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2">
         <v>1039351946</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="2">
         <v>1039351946</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="H22">
-        <v>1</v>
+      <c r="H22" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -1784,13 +1787,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2">
         <v>131249715</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="2">
         <v>131249715</v>
@@ -1799,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1840,18 +1843,18 @@
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2">
         <v>2470326492</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2">
         <v>2470326492</v>
@@ -1860,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -1877,13 +1880,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="10">
         <v>32075905</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="10">
         <v>32075905</v>
@@ -1892,10 +1895,10 @@
         <v>4</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="9">
         <v>2</v>
@@ -1912,7 +1915,7 @@
         <v>1012227440</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2">
         <v>1012227440</v>
@@ -1921,7 +1924,7 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1944,19 +1947,19 @@
         <v>1012234923</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2">
         <v>1012234923</v>
       </c>
       <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
         <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" t="s">
-        <v>35</v>
       </c>
       <c r="H28">
         <v>6</v>
@@ -1970,13 +1973,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2">
         <v>102342134</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2">
         <v>102342134</v>
@@ -1985,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H29">
         <v>4</v>
@@ -2005,7 +2008,7 @@
         <v>1032223563</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2">
         <v>1032223563</v>
@@ -2014,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2031,13 +2034,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2">
         <v>1338173424</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2">
         <v>1338173424</v>
@@ -2046,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31">
         <v>5</v>

</xml_diff>

<commit_message>
Nuevos cambios a la base de datos del Ejercicio de limpieza
</commit_message>
<xml_diff>
--- a/Dataset/EjercicioLimpieza.xlsx
+++ b/Dataset/EjercicioLimpieza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43736422-F23D-447F-B0F4-7EAB60A8BD02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3822AA10-8188-4522-977D-14D7CDB245E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>NA</t>
   </si>
@@ -124,9 +124,6 @@
     <t>uno</t>
   </si>
   <si>
-    <t>Cedula de ciudadania</t>
-  </si>
-  <si>
     <t>Tarjeta de identidad</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>Prom*Caridad</t>
   </si>
   <si>
-    <t>Tarjeta de extranjeria</t>
-  </si>
-  <si>
     <t># cédula</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>06 20 2019</t>
   </si>
   <si>
-    <t>encuestado el 15/12/15</t>
-  </si>
-  <si>
     <t>Feb 6 13</t>
   </si>
   <si>
@@ -203,6 +194,15 @@
   </si>
   <si>
     <t>10/18/2018 satisfactoria!</t>
+  </si>
+  <si>
+    <t>encuestado el 05/12/15</t>
+  </si>
+  <si>
+    <t>Cédula de ciudadanía</t>
+  </si>
+  <si>
+    <t>Tarjeta de extranjería</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1054,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1066,10 +1071,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -1079,13 +1084,13 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1096,7 +1101,7 @@
         <v>103586998</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D2" s="4">
         <v>103586998</v>
@@ -1128,7 +1133,7 @@
         <v>103587812</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>103587812</v>
@@ -1163,7 +1168,7 @@
         <v>100730671</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4">
         <v>100730671</v>
@@ -1198,7 +1203,7 @@
         <v>19355635</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4">
         <v>19355635</v>
@@ -1230,7 +1235,7 @@
         <v>103857245</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4">
         <v>103857245</v>
@@ -1262,7 +1267,7 @@
         <v>190730671</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4">
         <v>190730671</v>
@@ -1292,7 +1297,7 @@
         <v>123488986</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4">
         <v>123488986</v>
@@ -1307,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I8" s="1">
         <v>5</v>
@@ -1318,16 +1323,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4">
         <v>210216677</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4">
-        <v>210216677</v>
+        <v>210211126677</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1356,7 +1361,7 @@
         <v>39359318</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D10" s="4">
         <v>39359318</v>
@@ -1371,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -1388,7 +1393,7 @@
         <v>19355635</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4">
         <v>19355635</v>
@@ -1414,13 +1419,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4">
         <v>32321157</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4">
         <v>32321157</v>
@@ -1452,7 +1457,7 @@
         <v>127032350</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D13" s="4">
         <v>127032350</v>
@@ -1478,13 +1483,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4">
         <v>39350897</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4">
         <v>39350897</v>
@@ -1514,7 +1519,7 @@
         <v>60328769</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D15" s="4">
         <v>60328769</v>
@@ -1542,7 +1547,7 @@
         <v>1035874914</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D16" s="4">
         <v>1035874914</v>
@@ -1568,13 +1573,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4">
         <v>32075905</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D17" s="4">
         <v>32075905</v>
@@ -1600,13 +1605,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4">
         <v>1203870219</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D18" s="4">
         <v>1203870219</v>
@@ -1632,13 +1637,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4">
         <v>70320453</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4">
         <v>70320453</v>
@@ -1664,13 +1669,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4">
         <v>39350897</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="4">
         <v>39350897</v>
@@ -1700,7 +1705,7 @@
         <v>1040305449</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4">
         <v>1040305449</v>
@@ -1726,16 +1731,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4">
         <v>1039351946</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D22" s="4">
-        <v>1039351946</v>
+        <v>1039351942216</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
@@ -1745,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I22" s="1">
         <v>2</v>
@@ -1756,13 +1761,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="4">
         <v>131249715</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="4">
         <v>131249715</v>
@@ -1804,27 +1809,27 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1">
-        <v>5</v>
+        <v>999</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="1">
-        <v>2</v>
+      <c r="I24" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="4">
         <v>2470326492</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D25" s="4">
         <v>2470326492</v>
@@ -1850,13 +1855,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4">
         <v>32075905</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D26" s="4">
         <v>32075905</v>
@@ -1886,7 +1891,7 @@
         <v>1012227440</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D27" s="4">
         <v>1012227440</v>
@@ -1901,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="1">
-        <v>3</v>
+        <v>999</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
@@ -1912,13 +1917,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B28" s="4">
         <v>1012234923</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D28" s="4">
         <v>1012234923</v>
@@ -1944,13 +1949,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="4">
         <v>102342134</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D29" s="4">
         <v>102342134</v>
@@ -1980,7 +1985,7 @@
         <v>1032223563</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="4">
         <v>1032223563</v>
@@ -2006,13 +2011,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31" s="4">
         <v>1338173424</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="4">
         <v>1338173424</v>

</xml_diff>